<commit_message>
Ablaufplan ausgebessert, Projektstrukturplan fertiggestellt
</commit_message>
<xml_diff>
--- a/Projekt/Ablaufplan.xlsx
+++ b/Projekt/Ablaufplan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="132" windowWidth="23712" windowHeight="9792"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="23715" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>V 3.1</t>
   </si>
   <si>
-    <t>AP 4.0 Umsetzung</t>
-  </si>
-  <si>
     <t>V 4.1</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>offene Punkte + weiteres festlegen</t>
+  </si>
+  <si>
+    <t>AP 4.0 Abschluss</t>
   </si>
 </sst>
 </file>
@@ -297,15 +297,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -313,6 +304,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -323,6 +317,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,23 +522,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -574,23 +557,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -770,268 +736,268 @@
   <dimension ref="B1:AQ30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="43" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.375" customWidth="1"/>
+    <col min="4" max="43" width="4.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="14"/>
-      <c r="AJ1" s="14"/>
-      <c r="AK1" s="14"/>
-      <c r="AL1" s="14"/>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="14"/>
-      <c r="AQ1" s="14"/>
-    </row>
-    <row r="2" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="14"/>
-      <c r="AG2" s="14"/>
-      <c r="AH2" s="14"/>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="14"/>
-      <c r="AK2" s="14"/>
-      <c r="AL2" s="14"/>
-      <c r="AM2" s="14"/>
-      <c r="AN2" s="14"/>
-      <c r="AO2" s="14"/>
-      <c r="AP2" s="14"/>
-      <c r="AQ2" s="14"/>
-    </row>
-    <row r="4" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+    </row>
+    <row r="2" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="12"/>
+    </row>
+    <row r="4" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="D6" s="7" t="s">
+    <row r="6" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="D6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7" t="s">
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7" t="s">
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7" t="s">
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7" t="s">
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7" t="s">
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7"/>
-      <c r="AE6" s="7"/>
-      <c r="AF6" s="7" t="s">
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AG6" s="7"/>
-      <c r="AH6" s="7"/>
-      <c r="AI6" s="7"/>
-      <c r="AJ6" s="7" t="s">
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AK6" s="7"/>
-      <c r="AL6" s="7"/>
-      <c r="AM6" s="7"/>
-      <c r="AN6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO6" s="7"/>
-      <c r="AP6" s="7"/>
-      <c r="AQ6" s="7"/>
-    </row>
-    <row r="7" spans="2:43" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="7"/>
-      <c r="AD7" s="7"/>
-      <c r="AE7" s="7"/>
-      <c r="AF7" s="7"/>
-      <c r="AG7" s="7"/>
-      <c r="AH7" s="7"/>
-      <c r="AI7" s="7"/>
-      <c r="AJ7" s="7"/>
-      <c r="AK7" s="7"/>
-      <c r="AL7" s="7"/>
-      <c r="AM7" s="7"/>
-      <c r="AN7" s="7"/>
-      <c r="AO7" s="7"/>
-      <c r="AP7" s="7"/>
-      <c r="AQ7" s="7"/>
-    </row>
-    <row r="8" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+      <c r="AK6" s="9"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="9"/>
+      <c r="AQ6" s="9"/>
+    </row>
+    <row r="7" spans="2:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="9"/>
+    </row>
+    <row r="8" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="7"/>
-      <c r="AE8" s="7"/>
-      <c r="AF8" s="7"/>
-      <c r="AG8" s="7"/>
-      <c r="AH8" s="7"/>
-      <c r="AI8" s="7"/>
-      <c r="AJ8" s="7"/>
-      <c r="AK8" s="7"/>
-      <c r="AL8" s="7"/>
-      <c r="AM8" s="7"/>
-      <c r="AN8" s="7"/>
-      <c r="AO8" s="7"/>
-      <c r="AP8" s="7"/>
-      <c r="AQ8" s="7"/>
-    </row>
-    <row r="9" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="C8" s="13"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+      <c r="AN8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
+      <c r="AQ8" s="9"/>
+    </row>
+    <row r="9" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1074,12 +1040,12 @@
       <c r="AP9" s="1"/>
       <c r="AQ9" s="1"/>
     </row>
-    <row r="10" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1122,58 +1088,58 @@
       <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
     </row>
-    <row r="11" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
-      <c r="Z11" s="7"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="7"/>
-      <c r="AD11" s="7"/>
-      <c r="AE11" s="7"/>
-      <c r="AF11" s="7"/>
-      <c r="AG11" s="7"/>
-      <c r="AH11" s="7"/>
-      <c r="AI11" s="7"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
       <c r="AJ11" s="4"/>
       <c r="AK11" s="4"/>
       <c r="AL11" s="4"/>
       <c r="AM11" s="4"/>
-      <c r="AN11" s="7"/>
-      <c r="AO11" s="7"/>
-      <c r="AP11" s="7"/>
-      <c r="AQ11" s="7"/>
-    </row>
-    <row r="12" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="9"/>
+      <c r="AQ11" s="9"/>
+    </row>
+    <row r="12" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1216,12 +1182,12 @@
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
     </row>
-    <row r="13" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1264,12 +1230,12 @@
       <c r="AP13" s="1"/>
       <c r="AQ13" s="1"/>
     </row>
-    <row r="14" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1312,12 +1278,12 @@
       <c r="AP14" s="1"/>
       <c r="AQ14" s="1"/>
     </row>
-    <row r="15" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1360,12 +1326,12 @@
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
     </row>
-    <row r="16" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1408,12 +1374,12 @@
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
     </row>
-    <row r="17" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1456,58 +1422,58 @@
       <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
     </row>
-    <row r="18" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B18" s="12" t="s">
+    <row r="18" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="9"/>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="9"/>
-      <c r="AG18" s="10"/>
-      <c r="AH18" s="10"/>
-      <c r="AI18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="8"/>
+      <c r="AF18" s="6"/>
+      <c r="AG18" s="7"/>
+      <c r="AH18" s="7"/>
+      <c r="AI18" s="8"/>
       <c r="AJ18" s="5"/>
       <c r="AK18" s="5"/>
       <c r="AL18" s="5"/>
       <c r="AM18" s="5"/>
-      <c r="AN18" s="9"/>
-      <c r="AO18" s="10"/>
-      <c r="AP18" s="10"/>
-      <c r="AQ18" s="11"/>
-    </row>
-    <row r="19" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="AN18" s="6"/>
+      <c r="AO18" s="7"/>
+      <c r="AP18" s="7"/>
+      <c r="AQ18" s="8"/>
+    </row>
+    <row r="19" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1550,12 +1516,12 @@
       <c r="AP19" s="1"/>
       <c r="AQ19" s="1"/>
     </row>
-    <row r="20" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1598,12 +1564,12 @@
       <c r="AP20" s="1"/>
       <c r="AQ20" s="1"/>
     </row>
-    <row r="21" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1646,12 +1612,12 @@
       <c r="AP21" s="1"/>
       <c r="AQ21" s="1"/>
     </row>
-    <row r="22" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1694,12 +1660,12 @@
       <c r="AP22" s="1"/>
       <c r="AQ22" s="1"/>
     </row>
-    <row r="23" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1742,58 +1708,58 @@
       <c r="AP23" s="1"/>
       <c r="AQ23" s="1"/>
     </row>
-    <row r="24" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
+    <row r="24" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
-      <c r="Y24" s="7"/>
-      <c r="Z24" s="7"/>
-      <c r="AA24" s="7"/>
-      <c r="AB24" s="7"/>
-      <c r="AC24" s="7"/>
-      <c r="AD24" s="7"/>
-      <c r="AE24" s="7"/>
-      <c r="AF24" s="7"/>
-      <c r="AG24" s="7"/>
-      <c r="AH24" s="7"/>
-      <c r="AI24" s="7"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9"/>
+      <c r="AI24" s="9"/>
       <c r="AJ24" s="4"/>
       <c r="AK24" s="4"/>
       <c r="AL24" s="4"/>
       <c r="AM24" s="4"/>
-      <c r="AN24" s="7"/>
-      <c r="AO24" s="7"/>
-      <c r="AP24" s="7"/>
-      <c r="AQ24" s="7"/>
-    </row>
-    <row r="25" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="AN24" s="9"/>
+      <c r="AO24" s="9"/>
+      <c r="AP24" s="9"/>
+      <c r="AQ24" s="9"/>
+    </row>
+    <row r="25" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1836,58 +1802,58 @@
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
     </row>
-    <row r="26" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B26" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="10"/>
-      <c r="V26" s="10"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="9"/>
-      <c r="Y26" s="10"/>
-      <c r="Z26" s="10"/>
-      <c r="AA26" s="11"/>
-      <c r="AB26" s="9"/>
-      <c r="AC26" s="10"/>
-      <c r="AD26" s="10"/>
-      <c r="AE26" s="11"/>
-      <c r="AF26" s="9"/>
-      <c r="AG26" s="10"/>
-      <c r="AH26" s="10"/>
-      <c r="AI26" s="11"/>
+    <row r="26" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="8"/>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="7"/>
+      <c r="AD26" s="7"/>
+      <c r="AE26" s="8"/>
+      <c r="AF26" s="6"/>
+      <c r="AG26" s="7"/>
+      <c r="AH26" s="7"/>
+      <c r="AI26" s="8"/>
       <c r="AJ26" s="5"/>
       <c r="AK26" s="5"/>
       <c r="AL26" s="5"/>
       <c r="AM26" s="5"/>
-      <c r="AN26" s="9"/>
-      <c r="AO26" s="10"/>
-      <c r="AP26" s="10"/>
-      <c r="AQ26" s="11"/>
-    </row>
-    <row r="27" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="AN26" s="6"/>
+      <c r="AO26" s="7"/>
+      <c r="AP26" s="7"/>
+      <c r="AQ26" s="8"/>
+    </row>
+    <row r="27" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1930,12 +1896,12 @@
       <c r="AP27" s="1"/>
       <c r="AQ27" s="1"/>
     </row>
-    <row r="28" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1978,12 +1944,12 @@
       <c r="AP28" s="1"/>
       <c r="AQ28" s="1"/>
     </row>
-    <row r="29" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -2026,7 +1992,7 @@
       <c r="AP29" s="1"/>
       <c r="AQ29" s="1"/>
     </row>
-    <row r="30" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2072,6 +2038,63 @@
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="T11:W11"/>
+    <mergeCell ref="X11:AA11"/>
+    <mergeCell ref="AB11:AE11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="X7:AA7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="X8:AA8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="AN18:AQ18"/>
+    <mergeCell ref="AF7:AI7"/>
+    <mergeCell ref="AN7:AQ7"/>
+    <mergeCell ref="AB7:AE7"/>
+    <mergeCell ref="AB8:AE8"/>
+    <mergeCell ref="AF8:AI8"/>
+    <mergeCell ref="AN8:AQ8"/>
+    <mergeCell ref="AF11:AI11"/>
+    <mergeCell ref="AN11:AQ11"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="X18:AA18"/>
+    <mergeCell ref="AB18:AE18"/>
+    <mergeCell ref="AB24:AE24"/>
+    <mergeCell ref="X24:AA24"/>
+    <mergeCell ref="T24:W24"/>
+    <mergeCell ref="P24:S24"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="B1:AQ2"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="AN6:AQ6"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="X6:AA6"/>
+    <mergeCell ref="AB6:AE6"/>
+    <mergeCell ref="AF6:AI6"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="P18:S18"/>
+    <mergeCell ref="AF18:AI18"/>
     <mergeCell ref="AN26:AQ26"/>
     <mergeCell ref="AJ6:AM6"/>
     <mergeCell ref="AJ7:AM7"/>
@@ -2085,66 +2108,9 @@
     <mergeCell ref="X26:AA26"/>
     <mergeCell ref="AB26:AE26"/>
     <mergeCell ref="AF26:AI26"/>
-    <mergeCell ref="B1:AQ2"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="AN6:AQ6"/>
-    <mergeCell ref="B18:C18"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="X6:AA6"/>
-    <mergeCell ref="AB6:AE6"/>
-    <mergeCell ref="AF6:AI6"/>
-    <mergeCell ref="L18:O18"/>
-    <mergeCell ref="P18:S18"/>
     <mergeCell ref="AN24:AQ24"/>
     <mergeCell ref="AF24:AI24"/>
-    <mergeCell ref="AB24:AE24"/>
-    <mergeCell ref="X24:AA24"/>
-    <mergeCell ref="T24:W24"/>
-    <mergeCell ref="P24:S24"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="T18:W18"/>
-    <mergeCell ref="X18:AA18"/>
-    <mergeCell ref="AB18:AE18"/>
-    <mergeCell ref="AF18:AI18"/>
-    <mergeCell ref="AN18:AQ18"/>
-    <mergeCell ref="AF7:AI7"/>
-    <mergeCell ref="AN7:AQ7"/>
-    <mergeCell ref="AB7:AE7"/>
-    <mergeCell ref="AB8:AE8"/>
-    <mergeCell ref="AF8:AI8"/>
-    <mergeCell ref="AN8:AQ8"/>
-    <mergeCell ref="AF11:AI11"/>
-    <mergeCell ref="AN11:AQ11"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="X7:AA7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="X8:AA8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="P11:S11"/>
-    <mergeCell ref="T11:W11"/>
-    <mergeCell ref="X11:AA11"/>
-    <mergeCell ref="AB11:AE11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2158,7 +2124,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2170,7 +2136,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>